<commit_message>
UPDATE: excel file structure
</commit_message>
<xml_diff>
--- a/src/models/retriever_evaluation_results.xlsx
+++ b/src/models/retriever_evaluation_results.xlsx
@@ -1,84 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eduard_babayan/Documents/personal_projects/geoquery-ai/src/models/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8806A522-E24B-AD4C-BE28-D31172A3DB00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>Model Name</t>
-  </si>
-  <si>
-    <t>MRR Score</t>
-  </si>
-  <si>
-    <t>Evaluation Time (seconds)</t>
-  </si>
-  <si>
-    <t>Default Retriever</t>
-  </si>
-  <si>
-    <t>Artem V1 Retriever</t>
-  </si>
-  <si>
-    <t>Artem V2 Retriever</t>
-  </si>
-  <si>
-    <t>Artem V3 Retriever</t>
-  </si>
-  <si>
-    <t>Enhanced Retriever</t>
-  </si>
-  <si>
-    <t>Default Retriever with Decomposition</t>
-  </si>
-  <si>
-    <t>Default Retriever with Reranker</t>
-  </si>
-  <si>
-    <t>Advanced Retriever (No Rerank)</t>
-  </si>
-  <si>
-    <t>Advanced Retriever (With Rerank)</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -93,43 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -417,126 +420,183 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="34.5" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Model Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>MRR Score</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Accuracy Score</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Evaluation Time (seconds)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Default Retriever</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
         <v>0.5592307692307692</v>
       </c>
-      <c r="C2">
-        <v>42.135519027709961</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>0.40487179487179481</v>
-      </c>
-      <c r="C3">
-        <v>36.86270809173584</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>0.37564102564102558</v>
-      </c>
-      <c r="C4">
-        <v>39.089879989624023</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>0.39820512820512821</v>
-      </c>
-      <c r="C5">
-        <v>42.835125923156738</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6">
-        <v>0.44615384615384618</v>
-      </c>
-      <c r="C6">
-        <v>42.287403106689453</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7">
-        <v>0.58487179487179486</v>
-      </c>
-      <c r="C7">
-        <v>316.58823394775391</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8">
-        <v>0.66410256410256407</v>
-      </c>
-      <c r="C8">
-        <v>43.537690877914429</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9">
-        <v>0.41358974358974371</v>
-      </c>
-      <c r="C9">
-        <v>42.41418719291687</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10">
-        <v>0.73512820512820509</v>
-      </c>
-      <c r="C10">
-        <v>48.647010087966919</v>
+      <c r="C2" t="n">
+        <v>0.8153846153846154</v>
+      </c>
+      <c r="D2" t="n">
+        <v>47.16374588012695</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Default Retriever with Decomposition</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.5787179487179487</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.7846153846153846</v>
+      </c>
+      <c r="D3" t="n">
+        <v>370.905054807663</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Default Retriever with Reranker</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.6641025641025641</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.8615384615384616</v>
+      </c>
+      <c r="D4" t="n">
+        <v>45.9077000617981</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Artem V1 Retriever</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.3997435897435898</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.6153846153846154</v>
+      </c>
+      <c r="D5" t="n">
+        <v>40.21091890335083</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Artem V2 Retriever</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.3756410256410256</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.5538461538461539</v>
+      </c>
+      <c r="D6" t="n">
+        <v>45.12209391593933</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Artem V3 Retriever</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.4048717948717948</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.6307692307692307</v>
+      </c>
+      <c r="D7" t="n">
+        <v>38.10602498054504</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Enhanced Retriever</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.4461538461538462</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.676923076923077</v>
+      </c>
+      <c r="D8" t="n">
+        <v>42.75040102005005</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Advanced Retriever (No Rerank)</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.4135897435897437</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.5538461538461539</v>
+      </c>
+      <c r="D9" t="n">
+        <v>45.28295993804932</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Advanced Retriever (With Rerank)</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.7351282051282051</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.8153846153846154</v>
+      </c>
+      <c r="D10" t="n">
+        <v>51.39133906364441</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ADD: new models that use columns descriptions
</commit_message>
<xml_diff>
--- a/src/models/retriever_evaluation_results.xlsx
+++ b/src/models/retriever_evaluation_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -599,6 +599,70 @@
         <v>51.39133906364441</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Column Enhanced Basic</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.5089743589743591</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.6923076923076923</v>
+      </c>
+      <c r="D11" t="n">
+        <v>120.9329941272736</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Column Enhanced BM25 Emphasis</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.4717948717948718</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.5846153846153846</v>
+      </c>
+      <c r="D12" t="n">
+        <v>101.1998147964478</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Column Enhanced Vector Emphasis</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0.4869230769230769</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.6615384615384615</v>
+      </c>
+      <c r="D13" t="n">
+        <v>70.17123675346375</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Column Enhanced with Reranking</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.8615384615384616</v>
+      </c>
+      <c r="D14" t="n">
+        <v>68.3456130027771</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
ADD: new models based on default and advanced models with column improvements
</commit_message>
<xml_diff>
--- a/src/models/retriever_evaluation_results.xlsx
+++ b/src/models/retriever_evaluation_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -663,6 +663,86 @@
         <v>68.3456130027771</v>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Default with Columns (BM25 0.7-0.3)</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.4474358974358975</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="D15" t="n">
+        <v>52.1882152557373</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Default with Columns (Balanced 0.5-0.5)</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0.5487179487179488</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.8153846153846154</v>
+      </c>
+      <c r="D16" t="n">
+        <v>54.05382180213928</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Default with Columns (Vector 0.3-0.7)</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>0.6205128205128204</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.8307692307692308</v>
+      </c>
+      <c r="D17" t="n">
+        <v>55.41543316841125</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Advanced with Columns (No Rerank)</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0.4671794871794872</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.5692307692307692</v>
+      </c>
+      <c r="D18" t="n">
+        <v>61.1391978263855</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Advanced with Columns (With Rerank)</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>0.6735897435897436</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.8461538461538461</v>
+      </c>
+      <c r="D19" t="n">
+        <v>54.67233204841614</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
ADD: graph variations for base models
</commit_message>
<xml_diff>
--- a/src/models/retriever_evaluation_results.xlsx
+++ b/src/models/retriever_evaluation_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -887,6 +887,118 @@
         <v>41.736811876297</v>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>KG Default (Balanced 0.5-0.5)</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>0.4728205128205129</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.7076923076923077</v>
+      </c>
+      <c r="D29" t="n">
+        <v>3.811671018600464</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>KG Artem V1 Full (Balanced 0.5-0.5)</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>0.3069230769230769</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.6307692307692307</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.7538149356842041</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>KG Artem V2 Purpose+Insights (Balanced 0.5-0.5)</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>0.3430769230769231</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0.6615384615384615</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.740900993347168</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>KG Artem V3 Full (Balanced 0.5-0.5)</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>0.3069230769230769</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0.6307692307692307</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.7330317497253418</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>KG Artem V4 Minimal (Balanced 0.5-0.5)</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>0.3374358974358974</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0.6307692307692307</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.7192442417144775</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>KG Default (BM25 0.7-0.3)</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>0.4123076923076923</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.6923076923076923</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.7164630889892578</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>KG Default (Vector 0.3-0.7)</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>0.4587179487179487</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0.7230769230769231</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.7145400047302246</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
ADD: graph + questions
</commit_message>
<xml_diff>
--- a/src/models/retriever_evaluation_results.xlsx
+++ b/src/models/retriever_evaluation_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -894,13 +894,13 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.4728205128205129</v>
+        <v>0.4482051282051282</v>
       </c>
       <c r="C29" t="n">
         <v>0.7076923076923077</v>
       </c>
       <c r="D29" t="n">
-        <v>3.811671018600464</v>
+        <v>42.44780707359314</v>
       </c>
     </row>
     <row r="30">
@@ -910,13 +910,13 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.3069230769230769</v>
+        <v>0.3348717948717949</v>
       </c>
       <c r="C30" t="n">
-        <v>0.6307692307692307</v>
+        <v>0.6153846153846154</v>
       </c>
       <c r="D30" t="n">
-        <v>0.7538149356842041</v>
+        <v>42.16033387184143</v>
       </c>
     </row>
     <row r="31">
@@ -926,13 +926,13 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.3430769230769231</v>
+        <v>0.3617948717948718</v>
       </c>
       <c r="C31" t="n">
-        <v>0.6615384615384615</v>
+        <v>0.6</v>
       </c>
       <c r="D31" t="n">
-        <v>0.740900993347168</v>
+        <v>49.48245310783386</v>
       </c>
     </row>
     <row r="32">
@@ -942,13 +942,13 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.3069230769230769</v>
+        <v>0.3335897435897436</v>
       </c>
       <c r="C32" t="n">
-        <v>0.6307692307692307</v>
+        <v>0.6153846153846154</v>
       </c>
       <c r="D32" t="n">
-        <v>0.7330317497253418</v>
+        <v>60.65169501304626</v>
       </c>
     </row>
     <row r="33">
@@ -958,13 +958,13 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.3374358974358974</v>
+        <v>0.3597435897435897</v>
       </c>
       <c r="C33" t="n">
-        <v>0.6307692307692307</v>
+        <v>0.6</v>
       </c>
       <c r="D33" t="n">
-        <v>0.7192442417144775</v>
+        <v>42.70323395729065</v>
       </c>
     </row>
     <row r="34">
@@ -974,13 +974,13 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.4123076923076923</v>
+        <v>0.4102564102564103</v>
       </c>
       <c r="C34" t="n">
         <v>0.6923076923076923</v>
       </c>
       <c r="D34" t="n">
-        <v>0.7164630889892578</v>
+        <v>48.004723072052</v>
       </c>
     </row>
     <row r="35">
@@ -990,13 +990,29 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.4587179487179487</v>
+        <v>0.4269230769230769</v>
       </c>
       <c r="C35" t="n">
-        <v>0.7230769230769231</v>
+        <v>0.7076923076923077</v>
       </c>
       <c r="D35" t="n">
-        <v>0.7145400047302246</v>
+        <v>44.29169511795044</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>KG Default + Questions (Vector 0.3-0.7)</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>0.6197435897435897</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0.8153846153846154</v>
+      </c>
+      <c r="D36" t="n">
+        <v>48.57017016410828</v>
       </c>
     </row>
   </sheetData>

</xml_diff>